<commit_message>
feat: add 3 pc map
</commit_message>
<xml_diff>
--- a/asserts/coords_tracking/FALLARBOR TOWN coordinates.xlsx
+++ b/asserts/coords_tracking/FALLARBOR TOWN coordinates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SS\Documents\GitHub\pokemmo_py_auto\asserts\coords_tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22050FC4-5D30-4427-9B34-21C3CB336B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8CD727-8940-480C-9D70-2057C37E1FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="2">
   <si>
     <t>pc_in</t>
   </si>
@@ -393,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AL19" sqref="AL19"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="CD15" sqref="CD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.42578125" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -729,31 +729,31 @@
       <c r="CD2" s="1">
         <v>1</v>
       </c>
-      <c r="CE2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CF2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CG2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CH2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CI2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CJ2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CK2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CL2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CM2" s="1" t="s">
+      <c r="CE2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CF2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CG2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CH2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CI2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CJ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CK2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CL2" s="1">
+        <v>1</v>
+      </c>
+      <c r="CM2" s="1">
         <v>1</v>
       </c>
       <c r="CN2" s="1">
@@ -773,34 +773,34 @@
       <c r="A3" s="2">
         <v>3</v>
       </c>
-      <c r="CD3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CE3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CF3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CG3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CH3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CI3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CJ3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CK3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CL3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CM3" s="1" t="s">
+      <c r="CD3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CE3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CF3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CG3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CH3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CI3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CJ3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CK3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CL3" s="1">
+        <v>1</v>
+      </c>
+      <c r="CM3" s="1">
         <v>1</v>
       </c>
       <c r="CN3" s="1">
@@ -850,34 +850,34 @@
       <c r="BY4" s="1">
         <v>1</v>
       </c>
-      <c r="BZ4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CA4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CB4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CC4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CD4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CE4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CF4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CG4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CH4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CI4" s="1" t="s">
+      <c r="BZ4" s="1">
+        <v>1</v>
+      </c>
+      <c r="CA4" s="1">
+        <v>1</v>
+      </c>
+      <c r="CB4" s="1">
+        <v>1</v>
+      </c>
+      <c r="CC4" s="1">
+        <v>1</v>
+      </c>
+      <c r="CD4" s="1">
+        <v>1</v>
+      </c>
+      <c r="CE4" s="1">
+        <v>1</v>
+      </c>
+      <c r="CF4" s="1">
+        <v>1</v>
+      </c>
+      <c r="CG4" s="1">
+        <v>1</v>
+      </c>
+      <c r="CH4" s="1">
+        <v>1</v>
+      </c>
+      <c r="CI4" s="1">
         <v>1</v>
       </c>
       <c r="CN4" s="1">
@@ -987,34 +987,34 @@
       <c r="BY5" s="1">
         <v>1</v>
       </c>
-      <c r="BZ5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CA5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CB5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CC5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CD5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CE5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CF5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CG5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CH5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CI5" s="1" t="s">
+      <c r="BZ5" s="1">
+        <v>1</v>
+      </c>
+      <c r="CA5" s="1">
+        <v>1</v>
+      </c>
+      <c r="CB5" s="1">
+        <v>1</v>
+      </c>
+      <c r="CC5" s="1">
+        <v>1</v>
+      </c>
+      <c r="CD5" s="1">
+        <v>1</v>
+      </c>
+      <c r="CE5" s="1">
+        <v>1</v>
+      </c>
+      <c r="CF5" s="1">
+        <v>1</v>
+      </c>
+      <c r="CG5" s="1">
+        <v>1</v>
+      </c>
+      <c r="CH5" s="1">
+        <v>1</v>
+      </c>
+      <c r="CI5" s="1">
         <v>1</v>
       </c>
       <c r="CN5" s="1">
@@ -1214,25 +1214,25 @@
       <c r="BY6" s="1">
         <v>1</v>
       </c>
-      <c r="BZ6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CA6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CB6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CC6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CD6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CE6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CF6" s="1" t="s">
+      <c r="BZ6" s="1">
+        <v>1</v>
+      </c>
+      <c r="CA6" s="1">
+        <v>1</v>
+      </c>
+      <c r="CB6" s="1">
+        <v>1</v>
+      </c>
+      <c r="CC6" s="1">
+        <v>1</v>
+      </c>
+      <c r="CD6" s="1">
+        <v>1</v>
+      </c>
+      <c r="CE6" s="1">
+        <v>1</v>
+      </c>
+      <c r="CF6" s="1">
         <v>1</v>
       </c>
       <c r="CI6" s="1">
@@ -1423,19 +1423,19 @@
       <c r="BY7" s="1">
         <v>1</v>
       </c>
-      <c r="BZ7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CA7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CB7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CC7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="CD7" s="1" t="s">
+      <c r="BZ7" s="1">
+        <v>1</v>
+      </c>
+      <c r="CA7" s="1">
+        <v>1</v>
+      </c>
+      <c r="CB7" s="1">
+        <v>1</v>
+      </c>
+      <c r="CC7" s="1">
+        <v>1</v>
+      </c>
+      <c r="CD7" s="1">
         <v>1</v>
       </c>
       <c r="CE7" s="1">

</xml_diff>